<commit_message>
Log Book dan Burn Down Chart
</commit_message>
<xml_diff>
--- a/src/Log Book dan BurnDownChart/BurnDownChart.xlsx
+++ b/src/Log Book dan BurnDownChart/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Project</t>
   </si>
@@ -76,78 +76,6 @@
   </si>
   <si>
     <t>Start</t>
-  </si>
-  <si>
-    <t>Day 10</t>
-  </si>
-  <si>
-    <t>Day 9</t>
-  </si>
-  <si>
-    <t>Day 8</t>
-  </si>
-  <si>
-    <t>Day 7</t>
-  </si>
-  <si>
-    <t>Day 6</t>
-  </si>
-  <si>
-    <t>Day 5</t>
-  </si>
-  <si>
-    <t>Day 4</t>
-  </si>
-  <si>
-    <t>Day 3</t>
-  </si>
-  <si>
-    <t>Day 2</t>
-  </si>
-  <si>
-    <t>Day 1</t>
-  </si>
-  <si>
-    <t>My Project</t>
-  </si>
-  <si>
-    <t>Story 1</t>
-  </si>
-  <si>
-    <t>Story 2</t>
-  </si>
-  <si>
-    <t>Story 3</t>
-  </si>
-  <si>
-    <t>Story 4</t>
-  </si>
-  <si>
-    <t>Task 2.2</t>
-  </si>
-  <si>
-    <t>Task 3.1</t>
-  </si>
-  <si>
-    <t>Task 3.2</t>
-  </si>
-  <si>
-    <t>Task 3.3</t>
-  </si>
-  <si>
-    <t>Task 3.4</t>
-  </si>
-  <si>
-    <t>Task 4.1</t>
-  </si>
-  <si>
-    <t>Task 4.2</t>
-  </si>
-  <si>
-    <t>Task 4.3</t>
-  </si>
-  <si>
-    <t>Task 4.4</t>
   </si>
   <si>
     <t>Ideal - Remaining efforts in uninterrupted working hours</t>
@@ -162,19 +90,58 @@
     <t>www.goodoldmanoj.com</t>
   </si>
   <si>
-    <t>Penyembuhan albino</t>
+    <t>Pengenalan Albino</t>
   </si>
   <si>
-    <t>Gejala albino</t>
+    <t>Albino</t>
   </si>
   <si>
-    <t>Penyebab albino</t>
+    <t>Pengertian Albino</t>
   </si>
   <si>
-    <t>Pengertian albino</t>
+    <t>Penyebab Albino</t>
   </si>
   <si>
-    <t>Pengenalan Albino</t>
+    <t>Gejala Albino</t>
+  </si>
+  <si>
+    <t>Penyembuhan Albino</t>
+  </si>
+  <si>
+    <t>Kategori Albino</t>
+  </si>
+  <si>
+    <t>Albino Tirosinase Positif</t>
+  </si>
+  <si>
+    <t>Albino Tirosinase Negatif</t>
+  </si>
+  <si>
+    <t>Tipe Albino</t>
+  </si>
+  <si>
+    <t>Oculocutaneous Albinism</t>
+  </si>
+  <si>
+    <t>Ocular Albinism</t>
+  </si>
+  <si>
+    <t>Mitos Albino</t>
+  </si>
+  <si>
+    <t>Mitos Albino Pada Manusia</t>
+  </si>
+  <si>
+    <t>Albino Pada Hewan</t>
+  </si>
+  <si>
+    <t>Pengantar Albino Pada Hewan</t>
+  </si>
+  <si>
+    <t>Mengidentifikasi Albino Pada Hewan</t>
+  </si>
+  <si>
+    <t>Masalah Pada Hewan Albino</t>
   </si>
 </sst>
 </file>
@@ -278,12 +245,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
@@ -305,6 +269,14 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -316,7 +288,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="id-ID"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -325,7 +297,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr lang="en-US"/>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -347,45 +319,56 @@
             <c:v>Ideal burndown</c:v>
           </c:tx>
           <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US"/>
+                </a:pPr>
+                <a:endParaRPr lang="id-ID"/>
+              </a:p>
+            </c:txPr>
             <c:showVal val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$F$5:$O$5</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>dd\-mmm</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Day 10</c:v>
+                  <c:v>41785</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Day 9</c:v>
+                  <c:v>41786</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Day 8</c:v>
+                  <c:v>41787</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Day 7</c:v>
+                  <c:v>41788</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Day 6</c:v>
+                  <c:v>41789</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Day 5</c:v>
+                  <c:v>41790</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Day 4</c:v>
+                  <c:v>41792</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Day 3</c:v>
+                  <c:v>41793</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Day 2</c:v>
+                  <c:v>41794</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Day 1</c:v>
+                  <c:v>41795</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -394,31 +377,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>67.5</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.5</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.5</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.5</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -434,45 +417,56 @@
             <c:v>Actual burndown</c:v>
           </c:tx>
           <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US"/>
+                </a:pPr>
+                <a:endParaRPr lang="id-ID"/>
+              </a:p>
+            </c:txPr>
             <c:showVal val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Sheet1!$F$5:$O$5</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>dd\-mmm</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Day 10</c:v>
+                  <c:v>41785</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Day 9</c:v>
+                  <c:v>41786</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Day 8</c:v>
+                  <c:v>41787</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Day 7</c:v>
+                  <c:v>41788</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Day 6</c:v>
+                  <c:v>41789</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Day 5</c:v>
+                  <c:v>41790</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Day 4</c:v>
+                  <c:v>41792</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Day 3</c:v>
+                  <c:v>41793</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Day 2</c:v>
+                  <c:v>41794</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Day 1</c:v>
+                  <c:v>41795</c:v>
                 </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -481,19 +475,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>74</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -503,25 +497,35 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="57404416"/>
-        <c:axId val="67572480"/>
+        <c:axId val="69454464"/>
+        <c:axId val="69472640"/>
       </c:lineChart>
-      <c:catAx>
-        <c:axId val="57404416"/>
+      <c:dateAx>
+        <c:axId val="69454464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67572480"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US"/>
+            </a:pPr>
+            <a:endParaRPr lang="id-ID"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="69472640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-      </c:catAx>
+      </c:dateAx>
       <c:valAx>
-        <c:axId val="67572480"/>
+        <c:axId val="69472640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,7 +533,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="57404416"/>
+        <c:crossAx val="69454464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -537,12 +541,22 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US"/>
+          </a:pPr>
+          <a:endParaRPr lang="id-ID"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -870,28 +884,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="5" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16384" s="4" customFormat="1" ht="15.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="9" t="s">
-        <v>31</v>
+      <c r="E1" s="8" t="s">
+        <v>7</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -17269,7 +17284,7 @@
       <c r="XFC1" s="1"/>
       <c r="XFD1" s="1"/>
     </row>
-    <row r="2" spans="1:16384" s="6" customFormat="1" ht="17.25" customHeight="1">
+    <row r="2" spans="1:16384" s="5" customFormat="1" ht="17.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -33655,18 +33670,18 @@
       <c r="XFC2" s="1"/>
       <c r="XFD2" s="1"/>
     </row>
-    <row r="3" spans="1:16384" s="5" customFormat="1" ht="23.25">
+    <row r="3" spans="1:16384" s="4" customFormat="1" ht="23.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="8" t="s">
-        <v>30</v>
+      <c r="D3" s="7" t="s">
+        <v>6</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -50066,648 +50081,496 @@
     </row>
     <row r="5" spans="1:16384">
       <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>4</v>
+      <c r="F5" s="10">
+        <v>41785</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>5</v>
+      <c r="G5" s="10">
+        <v>41786</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>6</v>
+      <c r="H5" s="10">
+        <v>41787</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>7</v>
+      <c r="I5" s="10">
+        <v>41788</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>8</v>
+      <c r="J5" s="10">
+        <v>41789</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>9</v>
+      <c r="K5" s="10">
+        <v>41790</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>10</v>
+      <c r="L5" s="10">
+        <v>41792</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>11</v>
+      <c r="M5" s="10">
+        <v>41793</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>12</v>
+      <c r="N5" s="10">
+        <v>41794</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>13</v>
+      <c r="O5" s="10">
+        <v>41795</v>
       </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="P5" s="10">
+        <v>41796</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>41797</v>
+      </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:16384">
       <c r="A6" s="1"/>
-      <c r="B6" s="3" t="s">
-        <v>36</v>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>35</v>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
       </c>
-      <c r="E6" s="4">
-        <v>3</v>
-      </c>
-      <c r="F6" s="4">
-        <v>3</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
-        <v>0</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:16384">
       <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="4">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4">
-        <v>3</v>
-      </c>
-      <c r="G7" s="4">
-        <v>3</v>
-      </c>
-      <c r="H7" s="4">
-        <v>5</v>
-      </c>
-      <c r="I7" s="4">
-        <v>2</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:16384">
       <c r="A8" s="1"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>33</v>
+      <c r="E8" s="3">
+        <v>10</v>
       </c>
-      <c r="E8" s="4">
-        <v>3</v>
+      <c r="F8" s="3">
+        <v>8</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="3">
+        <v>6</v>
+      </c>
+      <c r="H8" s="3">
         <v>2</v>
       </c>
-      <c r="G8" s="4">
-        <v>3</v>
-      </c>
-      <c r="H8" s="4">
-        <v>2</v>
-      </c>
-      <c r="I8" s="4">
-        <v>2</v>
-      </c>
-      <c r="J8" s="4">
-        <v>0</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:16384">
       <c r="A9" s="1"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>32</v>
+      <c r="E9" s="3">
+        <v>8</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="3">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3">
         <v>3</v>
       </c>
-      <c r="F9" s="4">
-        <v>3</v>
+      <c r="H9" s="3">
+        <v>1</v>
       </c>
-      <c r="G9" s="4">
-        <v>8</v>
-      </c>
-      <c r="H9" s="4">
-        <v>8</v>
-      </c>
-      <c r="I9" s="4">
-        <v>7</v>
-      </c>
-      <c r="J9" s="4">
-        <v>3</v>
-      </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:16384">
       <c r="A10" s="1"/>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>16</v>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="4">
-        <v>8</v>
-      </c>
-      <c r="F10" s="4">
-        <v>8</v>
-      </c>
-      <c r="G10" s="4">
-        <v>8</v>
-      </c>
-      <c r="H10" s="4">
-        <v>8</v>
-      </c>
-      <c r="I10" s="4">
-        <v>8</v>
-      </c>
-      <c r="J10" s="4">
-        <v>7</v>
-      </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:16384">
       <c r="A11" s="1"/>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="4">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4">
-        <v>9</v>
-      </c>
-      <c r="G11" s="4">
-        <v>9</v>
-      </c>
-      <c r="H11" s="4">
-        <v>9</v>
-      </c>
-      <c r="I11" s="4">
-        <v>9</v>
-      </c>
-      <c r="J11" s="4">
-        <v>9</v>
-      </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:16384">
       <c r="A12" s="1"/>
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>21</v>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
       </c>
-      <c r="E12" s="4">
-        <v>5</v>
-      </c>
-      <c r="F12" s="4">
-        <v>5</v>
-      </c>
-      <c r="G12" s="4">
-        <v>5</v>
-      </c>
-      <c r="H12" s="4">
-        <v>5</v>
-      </c>
-      <c r="I12" s="4">
-        <v>5</v>
-      </c>
-      <c r="J12" s="4">
-        <v>5</v>
-      </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:16384">
       <c r="A13" s="1"/>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>7</v>
       </c>
-      <c r="F13" s="4">
-        <v>7</v>
+      <c r="F13" s="3">
+        <v>5</v>
       </c>
-      <c r="G13" s="4">
-        <v>7</v>
+      <c r="G13" s="3">
+        <v>2</v>
       </c>
-      <c r="H13" s="4">
-        <v>7</v>
+      <c r="H13" s="3">
+        <v>1</v>
       </c>
-      <c r="I13" s="4">
-        <v>7</v>
-      </c>
-      <c r="J13" s="4">
-        <v>7</v>
-      </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:16384">
       <c r="A14" s="1"/>
-      <c r="B14" s="3" t="s">
-        <v>14</v>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>20</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>17</v>
+      <c r="D14" s="2" t="s">
+        <v>21</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>23</v>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3">
+        <v>6</v>
       </c>
-      <c r="E14" s="4">
-        <v>3</v>
-      </c>
-      <c r="F14" s="4">
-        <v>3</v>
-      </c>
-      <c r="G14" s="4">
-        <v>3</v>
-      </c>
-      <c r="H14" s="4">
-        <v>3</v>
-      </c>
-      <c r="I14" s="4">
-        <v>3</v>
-      </c>
-      <c r="J14" s="4">
-        <v>3</v>
-      </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:16384">
       <c r="A15" s="1"/>
-      <c r="B15" s="3" t="s">
-        <v>14</v>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>18</v>
+      <c r="D15" s="2" t="s">
+        <v>23</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3">
         <v>8</v>
       </c>
-      <c r="F15" s="4">
-        <v>8</v>
-      </c>
-      <c r="G15" s="4">
-        <v>8</v>
-      </c>
-      <c r="H15" s="4">
-        <v>8</v>
-      </c>
-      <c r="I15" s="4">
-        <v>8</v>
-      </c>
-      <c r="J15" s="4">
-        <v>8</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:16384">
       <c r="A16" s="1"/>
-      <c r="B16" s="3" t="s">
-        <v>14</v>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>24</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3">
+        <v>8</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="4">
-        <v>6</v>
-      </c>
-      <c r="F16" s="4">
-        <v>6</v>
-      </c>
-      <c r="G16" s="4">
-        <v>6</v>
-      </c>
-      <c r="H16" s="4">
-        <v>6</v>
-      </c>
-      <c r="I16" s="4">
-        <v>6</v>
-      </c>
-      <c r="J16" s="4">
-        <v>6</v>
-      </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="1"/>
-      <c r="B17" s="3" t="s">
-        <v>14</v>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>25</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="4">
-        <v>8</v>
-      </c>
-      <c r="F17" s="4">
-        <v>8</v>
-      </c>
-      <c r="G17" s="4">
-        <v>8</v>
-      </c>
-      <c r="H17" s="4">
-        <v>8</v>
-      </c>
-      <c r="I17" s="4">
-        <v>8</v>
-      </c>
-      <c r="J17" s="4">
-        <v>8</v>
-      </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="1"/>
-      <c r="B18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="4">
-        <v>9</v>
-      </c>
-      <c r="F18" s="4">
-        <v>9</v>
-      </c>
-      <c r="G18" s="4">
-        <v>9</v>
-      </c>
-      <c r="H18" s="4">
-        <v>9</v>
-      </c>
-      <c r="I18" s="4">
-        <v>9</v>
-      </c>
-      <c r="J18" s="4">
-        <v>9</v>
-      </c>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="1"/>
-      <c r="B19" s="7" t="s">
-        <v>28</v>
+      <c r="B19" s="6" t="s">
+        <v>4</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="4">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3">
         <f>SUM(E6:E18)</f>
-        <v>75</v>
+        <v>25</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <f>E19-$E$19/10</f>
-        <v>67.5</v>
-      </c>
-      <c r="G19" s="4">
-        <f t="shared" ref="G19:O19" si="0">F19-$E$19/10</f>
-        <v>60</v>
-      </c>
-      <c r="H19" s="4">
-        <f t="shared" si="0"/>
-        <v>52.5</v>
-      </c>
-      <c r="I19" s="4">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="J19" s="4">
-        <f t="shared" si="0"/>
-        <v>37.5</v>
-      </c>
-      <c r="K19" s="4">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="L19" s="4">
-        <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
-      <c r="M19" s="4">
+      <c r="G19" s="3">
+        <f t="shared" ref="G19:Q19" si="0">F19-$E$19/10</f>
+        <v>20</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="I19" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="N19" s="4">
+      <c r="J19" s="3">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L19" s="3">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="O19" s="4">
+      <c r="M19" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="O19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
+      <c r="P19" s="3">
+        <f t="shared" si="0"/>
+        <v>-2.5</v>
+      </c>
+      <c r="Q19" s="3">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="1"/>
-      <c r="B20" s="7" t="s">
-        <v>29</v>
+      <c r="B20" s="6" t="s">
+        <v>5</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="4">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="3">
         <f>SUM(E6:E18)</f>
-        <v>75</v>
+        <v>25</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <f t="shared" ref="F20:J20" si="1">SUM(F6:F18)</f>
-        <v>74</v>
+        <v>18</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>11</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>4</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="3">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>22</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="3">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>0</v>
       </c>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>

</xml_diff>

<commit_message>
Log Book dan Burndown Chart
</commit_message>
<xml_diff>
--- a/src/Log Book dan BurnDownChart/BurnDownChart.xlsx
+++ b/src/Log Book dan BurnDownChart/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Project</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Masalah Pada Hewan Albino</t>
+  </si>
+  <si>
+    <t>Mitos Albino Pada Hewan</t>
   </si>
 </sst>
 </file>
@@ -372,39 +375,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$19:$O$19</c:f>
+              <c:f>Sheet1!$F$20:$O$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>42.3</c:v>
+                  <c:v>44.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.599999999999994</c:v>
+                  <c:v>39.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.899999999999991</c:v>
+                  <c:v>34.300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.199999999999992</c:v>
+                  <c:v>29.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.499999999999993</c:v>
+                  <c:v>24.500000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.799999999999994</c:v>
+                  <c:v>19.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.099999999999994</c:v>
+                  <c:v>14.700000000000008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.399999999999995</c:v>
+                  <c:v>9.8000000000000078</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.6999999999999948</c:v>
+                  <c:v>4.9000000000000075</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>7.1054273576010019E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -470,7 +473,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$20:$O$20</c:f>
+              <c:f>Sheet1!$F$21:$O$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -484,10 +487,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -497,11 +500,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="80015360"/>
-        <c:axId val="80016896"/>
+        <c:axId val="76804480"/>
+        <c:axId val="76806016"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="80015360"/>
+        <c:axId val="76804480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,13 +522,13 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80016896"/>
+        <c:crossAx val="76806016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="80016896"/>
+        <c:axId val="76806016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -533,7 +536,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="80015360"/>
+        <c:crossAx val="76804480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -556,7 +559,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -568,13 +571,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>514351</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -882,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD56"/>
+  <dimension ref="A1:XFC57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -896,7 +899,7 @@
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="4" customFormat="1" ht="15.75">
+    <row r="1" spans="1:16383" s="4" customFormat="1" ht="15.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -17282,9 +17285,8 @@
       <c r="XFA1" s="1"/>
       <c r="XFB1" s="1"/>
       <c r="XFC1" s="1"/>
-      <c r="XFD1" s="1"/>
     </row>
-    <row r="2" spans="1:16384" s="5" customFormat="1" ht="17.25" customHeight="1">
+    <row r="2" spans="1:16383" s="5" customFormat="1" ht="17.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -33668,9 +33670,8 @@
       <c r="XFA2" s="1"/>
       <c r="XFB2" s="1"/>
       <c r="XFC2" s="1"/>
-      <c r="XFD2" s="1"/>
     </row>
-    <row r="3" spans="1:16384" s="4" customFormat="1" ht="23.25">
+    <row r="3" spans="1:16383" s="4" customFormat="1" ht="23.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -50056,9 +50057,8 @@
       <c r="XFA3" s="1"/>
       <c r="XFB3" s="1"/>
       <c r="XFC3" s="1"/>
-      <c r="XFD3" s="1"/>
     </row>
-    <row r="4" spans="1:16384">
+    <row r="4" spans="1:16383">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -50079,7 +50079,7 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:16384">
+    <row r="5" spans="1:16383">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>0</v>
@@ -50132,7 +50132,7 @@
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:16384">
+    <row r="6" spans="1:16383">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -50159,7 +50159,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
     </row>
-    <row r="7" spans="1:16384">
+    <row r="7" spans="1:16383">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -50182,7 +50182,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:16384">
+    <row r="8" spans="1:16383">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -50213,7 +50213,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
     </row>
-    <row r="9" spans="1:16384">
+    <row r="9" spans="1:16383">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -50244,7 +50244,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
     </row>
-    <row r="10" spans="1:16384">
+    <row r="10" spans="1:16383">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -50269,7 +50269,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="1:16384">
+    <row r="11" spans="1:16383">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -50292,7 +50292,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="1:16384">
+    <row r="12" spans="1:16383">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -50317,7 +50317,7 @@
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="1:16384">
+    <row r="13" spans="1:16383">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -50348,7 +50348,7 @@
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="1:16384">
+    <row r="14" spans="1:16383">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
@@ -50358,15 +50358,17 @@
         <v>21</v>
       </c>
       <c r="E14" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
-      <c r="J14" s="3"/>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -50377,25 +50379,23 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:16384">
+    <row r="15" spans="1:16383">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3">
-        <v>8</v>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3">
+        <v>4</v>
       </c>
-      <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -50406,12 +50406,14 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:16384">
+    <row r="16" spans="1:16383">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="3">
         <v>8</v>
@@ -50420,7 +50422,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -50438,13 +50440,17 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3">
+        <v>8</v>
+      </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3">
+        <v>7</v>
+      </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -50460,7 +50466,9 @@
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -50479,125 +50487,125 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="1"/>
-      <c r="B19" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="3">
-        <f>SUM(E6:E18)</f>
-        <v>47</v>
-      </c>
-      <c r="F19" s="3">
-        <f>E19-$E$19/10</f>
-        <v>42.3</v>
-      </c>
-      <c r="G19" s="3">
-        <f t="shared" ref="G19:Q19" si="0">F19-$E$19/10</f>
-        <v>37.599999999999994</v>
-      </c>
-      <c r="H19" s="3">
-        <f t="shared" si="0"/>
-        <v>32.899999999999991</v>
-      </c>
-      <c r="I19" s="3">
-        <f t="shared" si="0"/>
-        <v>28.199999999999992</v>
-      </c>
-      <c r="J19" s="3">
-        <f t="shared" si="0"/>
-        <v>23.499999999999993</v>
-      </c>
-      <c r="K19" s="3">
-        <f t="shared" si="0"/>
-        <v>18.799999999999994</v>
-      </c>
-      <c r="L19" s="3">
-        <f t="shared" si="0"/>
-        <v>14.099999999999994</v>
-      </c>
-      <c r="M19" s="3">
-        <f t="shared" si="0"/>
-        <v>9.399999999999995</v>
-      </c>
-      <c r="N19" s="3">
-        <f t="shared" si="0"/>
-        <v>4.6999999999999948</v>
-      </c>
-      <c r="O19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="3">
-        <f t="shared" si="0"/>
-        <v>-4.7</v>
-      </c>
-      <c r="Q19" s="3">
-        <f t="shared" si="0"/>
-        <v>-9.4</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19">
       <c r="A20" s="1"/>
       <c r="B20" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="3">
-        <f>SUM(E6:E18)</f>
-        <v>47</v>
+        <f>SUM(E6:E19)</f>
+        <v>49</v>
       </c>
       <c r="F20" s="3">
-        <f t="shared" ref="F20:J20" si="1">SUM(F6:F18)</f>
-        <v>18</v>
+        <f>E20-$E$20/10</f>
+        <v>44.1</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <f t="shared" ref="G20:Q20" si="0">F20-$E$20/10</f>
+        <v>39.200000000000003</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>34.300000000000004</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" si="1"/>
-        <v>22</v>
+        <f t="shared" si="0"/>
+        <v>29.400000000000006</v>
       </c>
       <c r="J20" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>24.500000000000007</v>
       </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
+      <c r="K20" s="3">
+        <f t="shared" si="0"/>
+        <v>19.600000000000009</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" si="0"/>
+        <v>14.700000000000008</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="0"/>
+        <v>9.8000000000000078</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="0"/>
+        <v>4.9000000000000075</v>
+      </c>
+      <c r="O20" s="3">
+        <f t="shared" si="0"/>
+        <v>7.1054273576010019E-15</v>
+      </c>
+      <c r="P20" s="3">
+        <f t="shared" si="0"/>
+        <v>-4.8999999999999932</v>
+      </c>
+      <c r="Q20" s="3">
+        <f t="shared" si="0"/>
+        <v>-9.7999999999999936</v>
+      </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
+      <c r="B21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="3">
+        <f>SUM(E6:E19)</f>
+        <v>49</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" ref="F21:J21" si="1">SUM(F6:F19)</f>
+        <v>18</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
     </row>
@@ -51336,11 +51344,32 @@
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
     </row>
+    <row r="57" spans="1:19">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+    </row>
   </sheetData>
   <sheetProtection password="EF56" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
-    <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="D3:I3"/>
     <mergeCell ref="E1:H1"/>
   </mergeCells>

</xml_diff>

<commit_message>
logbook dan burndown chart
</commit_message>
<xml_diff>
--- a/src/Log Book dan BurnDownChart/BurnDownChart.xlsx
+++ b/src/Log Book dan BurnDownChart/BurnDownChart.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Project</t>
   </si>
@@ -156,7 +156,28 @@
     <t>Persilangan Albino</t>
   </si>
   <si>
-    <t>persilangan pada albino</t>
+    <t>Persilangan Pada Albino</t>
+  </si>
+  <si>
+    <t>Kelainan Mata Albino</t>
+  </si>
+  <si>
+    <t>Nystagmus</t>
+  </si>
+  <si>
+    <t>Strabismus</t>
+  </si>
+  <si>
+    <t>Fotosentivitas</t>
+  </si>
+  <si>
+    <t>Mata Silindris (Astigmatism)</t>
+  </si>
+  <si>
+    <t>Albino Pada Tanaman</t>
+  </si>
+  <si>
+    <t>Reed Wood Tree Albino</t>
   </si>
 </sst>
 </file>
@@ -321,6 +342,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -391,31 +413,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>71.099999999999994</c:v>
+                  <c:v>128.69999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.199999999999996</c:v>
+                  <c:v>114.39999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.3</c:v>
+                  <c:v>100.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47.4</c:v>
+                  <c:v>85.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.5</c:v>
+                  <c:v>71.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.6</c:v>
+                  <c:v>57.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.700000000000003</c:v>
+                  <c:v>42.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.800000000000002</c:v>
+                  <c:v>28.600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.9000000000000021</c:v>
+                  <c:v>14.300000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -492,22 +514,25 @@
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -517,11 +542,11 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="60080512"/>
-        <c:axId val="60082048"/>
+        <c:axId val="66380160"/>
+        <c:axId val="66381696"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="60080512"/>
+        <c:axId val="66380160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,13 +564,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60082048"/>
+        <c:crossAx val="66381696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="60082048"/>
+        <c:axId val="66381696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,13 +578,14 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="60080512"/>
+        <c:crossAx val="66380160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -575,7 +601,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -903,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -50168,9 +50194,7 @@
       <c r="G6" s="3">
         <v>0</v>
       </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -50289,10 +50313,16 @@
       <c r="D10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3">
+        <v>8</v>
+      </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="3">
+        <v>8</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -50312,10 +50342,16 @@
       <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3">
+        <v>7</v>
+      </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="3">
+        <v>7</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -50337,10 +50373,16 @@
       <c r="D12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3">
+        <v>6</v>
+      </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="3">
+        <v>6</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -50509,14 +50551,24 @@
       <c r="D18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3">
+        <v>8</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="I18" s="3">
+        <v>4</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -50548,7 +50600,9 @@
       <c r="L19" s="3">
         <v>1</v>
       </c>
-      <c r="M19" s="3"/>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
@@ -50575,9 +50629,11 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
-      <c r="M20" s="3"/>
+      <c r="M20" s="3">
+        <v>0</v>
+      </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
@@ -50588,17 +50644,27 @@
     <row r="21" spans="1:19">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
+      <c r="C21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="3">
+        <v>6</v>
+      </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="L21" s="3">
+        <v>6</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
@@ -50610,8 +50676,12 @@
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
+      <c r="D22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="3">
+        <v>8</v>
+      </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -50619,7 +50689,9 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="M22" s="3">
+        <v>6</v>
+      </c>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
@@ -50631,7 +50703,9 @@
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -50640,7 +50714,9 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="M23" s="3">
+        <v>7</v>
+      </c>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -50652,8 +50728,12 @@
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="3">
+        <v>7</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -50661,7 +50741,9 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="M24" s="3">
+        <v>5</v>
+      </c>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
@@ -50672,9 +50754,15 @@
     <row r="25" spans="1:19">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
+      <c r="C25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="3">
+        <v>8</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -50682,7 +50770,9 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="M25" s="3">
+        <v>6</v>
+      </c>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
@@ -50694,8 +50784,12 @@
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
+      <c r="D26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="3">
+        <v>6</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -50703,7 +50797,9 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
+      <c r="M26" s="3">
+        <v>4</v>
+      </c>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
@@ -50741,43 +50837,43 @@
       <c r="D28" s="8"/>
       <c r="E28" s="3">
         <f>SUM(E6:E27)</f>
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="F28" s="3">
         <f>E28-$E$28/10</f>
-        <v>71.099999999999994</v>
+        <v>128.69999999999999</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" ref="G28:Q28" si="0">F28-$E$28/10</f>
-        <v>63.199999999999996</v>
+        <v>114.39999999999999</v>
       </c>
       <c r="H28" s="3">
         <f t="shared" si="0"/>
-        <v>55.3</v>
+        <v>100.1</v>
       </c>
       <c r="I28" s="3">
         <f t="shared" si="0"/>
-        <v>47.4</v>
+        <v>85.8</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" si="0"/>
-        <v>39.5</v>
+        <v>71.5</v>
       </c>
       <c r="K28" s="3">
         <f t="shared" si="0"/>
-        <v>31.6</v>
+        <v>57.2</v>
       </c>
       <c r="L28" s="3">
         <f t="shared" si="0"/>
-        <v>23.700000000000003</v>
+        <v>42.900000000000006</v>
       </c>
       <c r="M28" s="3">
         <f t="shared" si="0"/>
-        <v>15.800000000000002</v>
+        <v>28.600000000000005</v>
       </c>
       <c r="N28" s="3">
         <f t="shared" si="0"/>
-        <v>7.9000000000000021</v>
+        <v>14.300000000000004</v>
       </c>
       <c r="O28" s="3">
         <f t="shared" si="0"/>
@@ -50785,11 +50881,11 @@
       </c>
       <c r="P28" s="3">
         <f t="shared" si="0"/>
-        <v>-7.9</v>
+        <v>-14.3</v>
       </c>
       <c r="Q28" s="3">
         <f t="shared" si="0"/>
-        <v>-15.8</v>
+        <v>-28.6</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -50803,7 +50899,7 @@
       <c r="D29" s="8"/>
       <c r="E29" s="3">
         <f t="shared" ref="E29:J29" si="1">SUM(E6:E27)</f>
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
@@ -50811,7 +50907,7 @@
       </c>
       <c r="G29" s="3">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="1"/>
@@ -50819,19 +50915,24 @@
       </c>
       <c r="I29" s="3">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K29" s="3">
-        <v>7</v>
+        <f>SUM(K6:K27)</f>
+        <v>8</v>
       </c>
       <c r="L29" s="3">
-        <v>6</v>
+        <f>SUM(L6:L27)</f>
+        <v>15</v>
       </c>
-      <c r="M29" s="3"/>
+      <c r="M29" s="3">
+        <f>SUM(M6:M27)</f>
+        <v>28</v>
+      </c>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>

</xml_diff>